<commit_message>
Removed 299 from crosswalk
Unknown conifer was listed twice. Fixes #15
</commit_message>
<xml_diff>
--- a/Your_species_codes.xlsx
+++ b/Your_species_codes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9588"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="136">
   <si>
     <t>FIA_code</t>
   </si>
@@ -423,24 +423,28 @@
   </si>
   <si>
     <t>XH</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>HX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -559,6 +563,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -594,6 +615,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -748,17 +786,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:I19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -772,7 +810,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -786,7 +824,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>14</v>
       </c>
@@ -797,7 +835,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>15</v>
       </c>
@@ -808,7 +846,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -822,7 +860,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>19</v>
       </c>
@@ -833,7 +871,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>20</v>
       </c>
@@ -844,7 +882,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>21</v>
       </c>
@@ -855,7 +893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>22</v>
       </c>
@@ -866,7 +904,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -880,7 +918,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>42</v>
       </c>
@@ -891,7 +929,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>50</v>
       </c>
@@ -902,7 +940,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>51</v>
       </c>
@@ -913,7 +951,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>52</v>
       </c>
@@ -924,7 +962,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>54</v>
       </c>
@@ -935,7 +973,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>55</v>
       </c>
@@ -946,7 +984,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>56</v>
       </c>
@@ -957,7 +995,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>62</v>
       </c>
@@ -968,7 +1006,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>64</v>
       </c>
@@ -979,7 +1017,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>65</v>
       </c>
@@ -990,7 +1028,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>66</v>
       </c>
@@ -1001,7 +1039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>72</v>
       </c>
@@ -1012,7 +1050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>73</v>
       </c>
@@ -1023,7 +1061,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>81</v>
       </c>
@@ -1034,7 +1072,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>92</v>
       </c>
@@ -1045,7 +1083,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>93</v>
       </c>
@@ -1056,7 +1094,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -1070,7 +1108,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>101</v>
       </c>
@@ -1081,7 +1119,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>102</v>
       </c>
@@ -1092,7 +1130,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>103</v>
       </c>
@@ -1103,7 +1141,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>104</v>
       </c>
@@ -1114,7 +1152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>108</v>
       </c>
@@ -1125,7 +1163,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>109</v>
       </c>
@@ -1136,7 +1174,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>113</v>
       </c>
@@ -1147,7 +1185,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>116</v>
       </c>
@@ -1158,7 +1196,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>117</v>
       </c>
@@ -1169,7 +1207,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -1183,7 +1221,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>120</v>
       </c>
@@ -1194,7 +1232,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>122</v>
       </c>
@@ -1205,7 +1243,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>124</v>
       </c>
@@ -1216,7 +1254,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>127</v>
       </c>
@@ -1227,7 +1265,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>130</v>
       </c>
@@ -1238,7 +1276,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>133</v>
       </c>
@@ -1249,7 +1287,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>137</v>
       </c>
@@ -1260,7 +1298,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>142</v>
       </c>
@@ -1271,7 +1309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>201</v>
       </c>
@@ -1282,7 +1320,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -1296,7 +1334,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>211</v>
       </c>
@@ -1307,7 +1345,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>212</v>
       </c>
@@ -1318,7 +1356,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>231</v>
       </c>
@@ -1329,7 +1367,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -1343,7 +1381,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>251</v>
       </c>
@@ -1354,7 +1392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -1368,7 +1406,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -1382,7 +1420,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
       <c r="B55">
         <v>298</v>
       </c>
@@ -1393,202 +1434,202 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>123</v>
+      </c>
       <c r="B56">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>123</v>
-      </c>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D57" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D58" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D59" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D60" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
       <c r="B63">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C63" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D63" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>126</v>
-      </c>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D66" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D67" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68">
-        <v>375</v>
+        <v>431</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D68" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69">
-        <v>431</v>
+        <v>475</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D69" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70">
-        <v>475</v>
+        <v>492</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D70" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D71" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D72" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C73" t="s">
         <v>72</v>
@@ -1597,42 +1638,42 @@
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D74" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D75" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76">
-        <v>547</v>
+        <v>590</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D76" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C77" t="s">
         <v>75</v>
@@ -1641,433 +1682,439 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="C78" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D78" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C79" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D79" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C80" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D80" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="C81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D81" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>129</v>
+      </c>
       <c r="B82">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="C82" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D82" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>129</v>
-      </c>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B83">
-        <v>631</v>
+        <v>660</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D83" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B84">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C84" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D84" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B85">
-        <v>661</v>
+        <v>730</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D85" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B86">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C86" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D86" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B87">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="C87" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D87" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>122</v>
+      </c>
       <c r="B88">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C88" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D88" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>122</v>
-      </c>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B89">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C89" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D89" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90">
-        <v>748</v>
-      </c>
-      <c r="C90" t="s">
-        <v>87</v>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B90" s="1">
+        <v>755</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D90" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="1">
-        <v>755</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>88</v>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>756</v>
+      </c>
+      <c r="C91" t="s">
+        <v>89</v>
       </c>
       <c r="D91" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B92">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C92" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D92" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>134</v>
+      </c>
       <c r="B93">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C93" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D93" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B94">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="C94" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D94" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B95">
-        <v>763</v>
+        <v>768</v>
       </c>
       <c r="C95" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D95" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B96">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="C96" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D96" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97">
-        <v>771</v>
+        <v>801</v>
       </c>
       <c r="C97" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D97" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D98" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D99" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="C100" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D100" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="C101" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D101" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D102" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="C103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D103" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D104" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105">
-        <v>826</v>
+        <v>839</v>
       </c>
       <c r="C105" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D105" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106">
-        <v>839</v>
+        <v>901</v>
       </c>
       <c r="C106" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D106" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107">
-        <v>901</v>
+        <v>920</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D107" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C108" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D108" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="C109" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D109" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D110" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C111" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D111" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112">
-        <v>929</v>
+        <v>981</v>
       </c>
       <c r="C112" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D112" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B113">
-        <v>981</v>
+        <v>990</v>
       </c>
       <c r="C113" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D113" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B114">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="C114" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D114" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>132</v>
+      </c>
       <c r="B115">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C115" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D115" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B116">
         <v>998</v>
@@ -2079,7 +2126,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B117">
         <v>999</v>
       </c>

</xml_diff>